<commit_message>
Changes of users id
</commit_message>
<xml_diff>
--- a/Input_sheet_V2.xlsx
+++ b/Input_sheet_V2.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Execution_Sheet" sheetId="5" r:id="rId1"/>
     <sheet name="Execution_Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Validation part" sheetId="4" r:id="rId3"/>
+    <sheet name="Credentials" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="210">
   <si>
     <t>Execution</t>
   </si>
@@ -559,12 +560,99 @@
   </si>
   <si>
     <t>Call Home for Less</t>
+  </si>
+  <si>
+    <t>/cluster/storage/no-backup/ccn/CcnStorage1/CCNCDR44/archive/</t>
+  </si>
+  <si>
+    <t>CCNtasuser@123</t>
+  </si>
+  <si>
+    <t>tasuser</t>
+  </si>
+  <si>
+    <t>10.95.213.132</t>
+  </si>
+  <si>
+    <t>CCN1</t>
+  </si>
+  <si>
+    <t>/cluster/storage/no-backup/ccn/CcnStorage0/CCNCDR44/archive/</t>
+  </si>
+  <si>
+    <t>CCN0</t>
+  </si>
+  <si>
+    <t>/var/opt/air/datarecords/backup_CDR/</t>
+  </si>
+  <si>
+    <t>Ericssondu@123</t>
+  </si>
+  <si>
+    <t>10.95.214.166</t>
+  </si>
+  <si>
+    <t>AIR</t>
+  </si>
+  <si>
+    <t>/home/tasuser</t>
+  </si>
+  <si>
+    <t>10.95.214.22</t>
+  </si>
+  <si>
+    <t>OCC2</t>
+  </si>
+  <si>
+    <t>10.95.214.21</t>
+  </si>
+  <si>
+    <t>OCC1</t>
+  </si>
+  <si>
+    <t>/var/opt/fds/CDR/archive/</t>
+  </si>
+  <si>
+    <t>10.95.214.6</t>
+  </si>
+  <si>
+    <t>SDP</t>
+  </si>
+  <si>
+    <t>/data/fdp/logs/defaultCircle</t>
+  </si>
+  <si>
+    <t>VenuReddyGaddam</t>
+  </si>
+  <si>
+    <t>10.95.214.72</t>
+  </si>
+  <si>
+    <t>CIS</t>
+  </si>
+  <si>
+    <t>Wait_Time</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>User_Name</t>
+  </si>
+  <si>
+    <t>IP_HostName</t>
+  </si>
+  <si>
+    <t>Unix_System</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -614,7 +702,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,6 +719,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -717,7 +811,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -766,6 +860,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1073,36 +1168,36 @@
   <dimension ref="A1:Z101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="32.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.90625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.90625" customWidth="1"/>
-    <col min="11" max="11" width="16.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="26.1796875" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.140625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="5" customFormat="1">
@@ -1570,417 +1665,417 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="26:26" ht="15" thickBot="1">
+    <row r="18" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z18" s="21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="26:26" ht="15" thickBot="1">
+    <row r="19" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z19" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="26:26" ht="15" thickBot="1">
+    <row r="20" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z20" s="23" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="26:26" ht="15" thickBot="1">
+    <row r="21" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z21" s="23" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="26:26" ht="15" thickBot="1">
+    <row r="22" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z22" s="23" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="26:26" ht="15" thickBot="1">
+    <row r="23" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z23" s="23" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="26:26" ht="15" thickBot="1">
+    <row r="24" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z24" s="23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="26:26" ht="15" thickBot="1">
+    <row r="25" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z25" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="26:26" ht="15" thickBot="1">
+    <row r="26" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z26" s="24" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="26:26" ht="15" thickBot="1">
+    <row r="27" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z27" s="24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="26:26" ht="15" thickBot="1">
+    <row r="28" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z28" s="24" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="26:26" ht="15" thickBot="1">
+    <row r="29" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z29" s="24" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="26:26" ht="15" thickBot="1">
+    <row r="30" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z30" s="24" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="26:26" ht="15" thickBot="1">
+    <row r="31" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z31" s="24" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="26:26" ht="15" thickBot="1">
+    <row r="32" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z32" s="24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="26:26" ht="15" thickBot="1">
+    <row r="33" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z33" s="24" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="26:26" ht="15" thickBot="1">
+    <row r="34" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z34" s="24" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="26:26" ht="15" thickBot="1">
+    <row r="35" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z35" s="24" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="26:26" ht="15" thickBot="1">
+    <row r="36" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z36" s="24" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="26:26" ht="15" thickBot="1">
+    <row r="37" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z37" s="24" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="26:26" ht="15" thickBot="1">
+    <row r="38" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z38" s="24" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="26:26" ht="15" thickBot="1">
+    <row r="39" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z39" s="24" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="26:26" ht="15" thickBot="1">
+    <row r="40" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z40" s="24" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="26:26" ht="15" thickBot="1">
+    <row r="41" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z41" s="24" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="26:26" ht="15" thickBot="1">
+    <row r="42" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z42" s="24" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="26:26" ht="15" thickBot="1">
+    <row r="43" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z43" s="24" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="26:26" ht="15" thickBot="1">
+    <row r="44" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z44" s="24" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="26:26" ht="15" thickBot="1">
+    <row r="45" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z45" s="24" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="26:26" ht="15" thickBot="1">
+    <row r="46" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z46" s="24" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="26:26" ht="15" thickBot="1">
+    <row r="47" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z47" s="24" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="26:26" ht="15" thickBot="1">
+    <row r="48" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z48" s="24" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="26:26" ht="15" thickBot="1">
+    <row r="49" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z49" s="24" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="26:26" ht="15" thickBot="1">
+    <row r="50" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z50" s="24" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="26:26" ht="15" thickBot="1">
+    <row r="51" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z51" s="24" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="26:26" ht="15" thickBot="1">
+    <row r="52" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z52" s="24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="26:26" ht="15" thickBot="1">
+    <row r="53" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z53" s="24" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="54" spans="26:26" ht="15" thickBot="1">
+    <row r="54" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z54" s="24" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="26:26" ht="15" thickBot="1">
+    <row r="55" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z55" s="24" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="26:26" ht="15" thickBot="1">
+    <row r="56" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z56" s="24" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="26:26" ht="15" thickBot="1">
+    <row r="57" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z57" s="24" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="26:26" ht="15" thickBot="1">
+    <row r="58" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z58" s="24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="59" spans="26:26" ht="15" thickBot="1">
+    <row r="59" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z59" s="24" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="26:26" ht="15" thickBot="1">
+    <row r="60" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z60" s="24" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="26:26" ht="15" thickBot="1">
+    <row r="61" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z61" s="24" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="62" spans="26:26" ht="15" thickBot="1">
+    <row r="62" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z62" s="24" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="63" spans="26:26" ht="15" thickBot="1">
+    <row r="63" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z63" s="24" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="64" spans="26:26" ht="15" thickBot="1">
+    <row r="64" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z64" s="24" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="26:26" ht="15" thickBot="1">
+    <row r="65" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z65" s="24" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="66" spans="26:26" ht="15" thickBot="1">
+    <row r="66" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z66" s="24" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="26:26" ht="15" thickBot="1">
+    <row r="67" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z67" s="24" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="26:26" ht="15" thickBot="1">
+    <row r="68" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z68" s="24" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="26:26" ht="15" thickBot="1">
+    <row r="69" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z69" s="24" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="70" spans="26:26" ht="15" thickBot="1">
+    <row r="70" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z70" s="24" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="71" spans="26:26" ht="15" thickBot="1">
+    <row r="71" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z71" s="24" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="72" spans="26:26" ht="15" thickBot="1">
+    <row r="72" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z72" s="24" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="73" spans="26:26" ht="15" thickBot="1">
+    <row r="73" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z73" s="24" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="74" spans="26:26" ht="15" thickBot="1">
+    <row r="74" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z74" s="24" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="75" spans="26:26" ht="15" thickBot="1">
+    <row r="75" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z75" s="24" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="76" spans="26:26" ht="15" thickBot="1">
+    <row r="76" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z76" s="24" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="77" spans="26:26" ht="15" thickBot="1">
+    <row r="77" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z77" s="24" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="78" spans="26:26" ht="15" thickBot="1">
+    <row r="78" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z78" s="24" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="79" spans="26:26" ht="15" thickBot="1">
+    <row r="79" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z79" s="24" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="80" spans="26:26" ht="15" thickBot="1">
+    <row r="80" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z80" s="24" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="26:26" ht="15" thickBot="1">
+    <row r="81" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z81" s="24" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="82" spans="26:26" ht="15" thickBot="1">
+    <row r="82" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z82" s="24" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="26:26" ht="15" thickBot="1">
+    <row r="83" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z83" s="24" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="26:26" ht="15" thickBot="1">
+    <row r="84" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z84" s="24" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="85" spans="26:26" ht="15" thickBot="1">
+    <row r="85" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z85" s="24" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="26:26" ht="15" thickBot="1">
+    <row r="86" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z86" s="24" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="87" spans="26:26" ht="15" thickBot="1">
+    <row r="87" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z87" s="24" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="88" spans="26:26" ht="15" thickBot="1">
+    <row r="88" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z88" s="24" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="89" spans="26:26" ht="15" thickBot="1">
+    <row r="89" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z89" s="24" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="90" spans="26:26" ht="15" thickBot="1">
+    <row r="90" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z90" s="24" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="91" spans="26:26" ht="15" thickBot="1">
+    <row r="91" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z91" s="24" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="92" spans="26:26" ht="15" thickBot="1">
+    <row r="92" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z92" s="24" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="93" spans="26:26" ht="15" thickBot="1">
+    <row r="93" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z93" s="24" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="94" spans="26:26" ht="15" thickBot="1">
+    <row r="94" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z94" s="24" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="95" spans="26:26" ht="15" thickBot="1">
+    <row r="95" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z95" s="24" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="96" spans="26:26" ht="15" thickBot="1">
+    <row r="96" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z96" s="24" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="97" spans="26:26" ht="15" thickBot="1">
+    <row r="97" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z97" s="24" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="98" spans="26:26" ht="15" thickBot="1">
+    <row r="98" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z98" s="24" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="99" spans="26:26" ht="15" thickBot="1">
+    <row r="99" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z99" s="24" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="100" spans="26:26" ht="15" thickBot="1">
+    <row r="100" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z100" s="24" t="s">
         <v>178</v>
       </c>
@@ -2030,24 +2125,24 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="26.1796875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="17.54296875" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="27.90625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="15.36328125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="19.90625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="15.36328125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="15.54296875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="27.85546875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="5" customFormat="1">
@@ -2442,14 +2537,14 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="3.90625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" customWidth="1"/>
-    <col min="12" max="12" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="5:13">
@@ -2722,4 +2817,186 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" t="s">
+        <v>186</v>
+      </c>
+      <c r="F7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
code after cis new node
</commit_message>
<xml_diff>
--- a/Input_sheet_V2.xlsx
+++ b/Input_sheet_V2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Execution_Sheet" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="211">
   <si>
     <t>Execution</t>
   </si>
@@ -619,15 +619,6 @@
     <t>SDP</t>
   </si>
   <si>
-    <t>/data/fdp/logs/defaultCircle</t>
-  </si>
-  <si>
-    <t>VenuReddyGaddam</t>
-  </si>
-  <si>
-    <t>10.95.214.72</t>
-  </si>
-  <si>
     <t>CIS</t>
   </si>
   <si>
@@ -647,6 +638,18 @@
   </si>
   <si>
     <t>Unix_System</t>
+  </si>
+  <si>
+    <t>10.95.214.9</t>
+  </si>
+  <si>
+    <t>atos</t>
+  </si>
+  <si>
+    <t>ericsson</t>
+  </si>
+  <si>
+    <t>/data/edr_enrichment/sftpcompleted</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -2823,8 +2826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2838,42 +2841,42 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="26" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="E2" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="F2">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2893,7 +2896,7 @@
         <v>197</v>
       </c>
       <c r="F3">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2913,7 +2916,7 @@
         <v>192</v>
       </c>
       <c r="F4">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2953,7 +2956,7 @@
         <v>188</v>
       </c>
       <c r="F6">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2973,7 +2976,7 @@
         <v>186</v>
       </c>
       <c r="F7">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">

</xml_diff>

<commit_message>
Fix for MVN run
</commit_message>
<xml_diff>
--- a/Input_sheet_V2.xlsx
+++ b/Input_sheet_V2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6480"/>
   </bookViews>
   <sheets>
     <sheet name="Execution_Sheet" sheetId="5" r:id="rId1"/>
@@ -1171,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1583,7 +1583,7 @@
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
@@ -2303,7 +2303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
first commit after api
</commit_message>
<xml_diff>
--- a/Input_sheet_V2.xlsx
+++ b/Input_sheet_V2.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6480" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Execution_Sheet" sheetId="5" r:id="rId1"/>
     <sheet name="Credentials" sheetId="6" r:id="rId2"/>
+    <sheet name="API_Data" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="273">
   <si>
     <t>Execution</t>
   </si>
@@ -681,13 +682,166 @@
   </si>
   <si>
     <t>device2</t>
+  </si>
+  <si>
+    <t>Request_Name</t>
+  </si>
+  <si>
+    <t>GetOffers</t>
+  </si>
+  <si>
+    <t>Execution Control</t>
+  </si>
+  <si>
+    <t>TestCase_ID</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>TC_009</t>
+  </si>
+  <si>
+    <t>TC_010</t>
+  </si>
+  <si>
+    <t>GetAccountDetails</t>
+  </si>
+  <si>
+    <t>DeleteOffer</t>
+  </si>
+  <si>
+    <t>UpdateOffer</t>
+  </si>
+  <si>
+    <t>UpdateDA</t>
+  </si>
+  <si>
+    <t>DeleteDA</t>
+  </si>
+  <si>
+    <t>GetBalanceAndDate</t>
+  </si>
+  <si>
+    <t>AddPAM</t>
+  </si>
+  <si>
+    <t>ReduceDA</t>
+  </si>
+  <si>
+    <t>AddDifferentDA</t>
+  </si>
+  <si>
+    <t>Parameter1</t>
+  </si>
+  <si>
+    <t>Value1</t>
+  </si>
+  <si>
+    <t>Parameter2</t>
+  </si>
+  <si>
+    <t>Value2</t>
+  </si>
+  <si>
+    <t>Parameter3</t>
+  </si>
+  <si>
+    <t>Value3</t>
+  </si>
+  <si>
+    <t>Parameter4</t>
+  </si>
+  <si>
+    <t>Value4</t>
+  </si>
+  <si>
+    <t>Parameter5</t>
+  </si>
+  <si>
+    <t>Value5</t>
+  </si>
+  <si>
+    <t>Parameter6</t>
+  </si>
+  <si>
+    <t>Value6</t>
+  </si>
+  <si>
+    <t>Parameter7</t>
+  </si>
+  <si>
+    <t>Value7</t>
+  </si>
+  <si>
+    <t>Parameter8</t>
+  </si>
+  <si>
+    <t>Value8</t>
+  </si>
+  <si>
+    <t>Parameter9</t>
+  </si>
+  <si>
+    <t>Value9</t>
+  </si>
+  <si>
+    <t>Parameter10</t>
+  </si>
+  <si>
+    <t>Value10</t>
+  </si>
+  <si>
+    <t>subscriberNumber</t>
+  </si>
+  <si>
+    <t>offerID</t>
+  </si>
+  <si>
+    <t>transactionCurrency</t>
+  </si>
+  <si>
+    <t>AED</t>
+  </si>
+  <si>
+    <t>dedicatedAccountID</t>
+  </si>
+  <si>
+    <t>adjustmentAmountRelative</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>dedicatedAccountUnitType</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>pamServiceID</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>pamClassID</t>
+  </si>
+  <si>
+    <t>scheduleID</t>
+  </si>
+  <si>
+    <t>-64</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -732,8 +886,23 @@
       <sz val="9"/>
       <name val="Ericsson Hilda"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -755,6 +924,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -827,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -868,6 +1049,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1174,37 +1360,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" style="11" customWidth="1"/>
-    <col min="7" max="7" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.90625" customWidth="1"/>
-    <col min="11" max="11" width="16.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="26.1796875" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="17.54296875" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="27.90625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7265625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="19.90625" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="15.7265625" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="15.54296875" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="38.453125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="26.140625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="27.85546875" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="19.85546875" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="38.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="5" customFormat="1">
@@ -1670,602 +1856,602 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="26:26" ht="15" thickBot="1">
+    <row r="18" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z18" s="17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="26:26" ht="15" thickBot="1">
+    <row r="19" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z19" s="18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="26:26" ht="15" thickBot="1">
+    <row r="20" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z20" s="19" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="26:26" ht="15" thickBot="1">
+    <row r="21" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z21" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="26:26" ht="15" thickBot="1">
+    <row r="22" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z22" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="26:26" ht="15" thickBot="1">
+    <row r="23" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z23" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="26:26" ht="15" thickBot="1">
+    <row r="24" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z24" s="19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="26:26" ht="15" thickBot="1">
+    <row r="25" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z25" s="19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="26:26" ht="15" thickBot="1">
+    <row r="26" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z26" s="20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="26:26" ht="15" thickBot="1">
+    <row r="27" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z27" s="20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="26:26" ht="15" thickBot="1">
+    <row r="28" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z28" s="20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="26:26" ht="15" thickBot="1">
+    <row r="29" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z29" s="20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="26:26" ht="15" thickBot="1">
+    <row r="30" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z30" s="20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="26:26" ht="15" thickBot="1">
+    <row r="31" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z31" s="20" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="26:26" ht="15" thickBot="1">
+    <row r="32" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z32" s="20" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="26:26" ht="15" thickBot="1">
+    <row r="33" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z33" s="20" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="26:26" ht="15" thickBot="1">
+    <row r="34" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z34" s="20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="26:26" ht="15" thickBot="1">
+    <row r="35" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z35" s="20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="26:26" ht="15" thickBot="1">
+    <row r="36" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z36" s="20" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="26:26" ht="15" thickBot="1">
+    <row r="37" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z37" s="20" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="26:26" ht="15" thickBot="1">
+    <row r="38" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z38" s="20" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="26:26" ht="15" thickBot="1">
+    <row r="39" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z39" s="20" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="26:26" ht="15" thickBot="1">
+    <row r="40" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z40" s="20" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="26:26" ht="15" thickBot="1">
+    <row r="41" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z41" s="20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="26:26" ht="15" thickBot="1">
+    <row r="42" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z42" s="20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="26:26" ht="15" thickBot="1">
+    <row r="43" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z43" s="20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="26:26" ht="15" thickBot="1">
+    <row r="44" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z44" s="20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="26:26" ht="15" thickBot="1">
+    <row r="45" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z45" s="20" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="26:26" ht="15" thickBot="1">
+    <row r="46" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z46" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="26:26" ht="15" thickBot="1">
+    <row r="47" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z47" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="26:26" ht="15" thickBot="1">
+    <row r="48" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z48" s="20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="26:26" ht="15" thickBot="1">
+    <row r="49" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z49" s="20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="26:26" ht="15" thickBot="1">
+    <row r="50" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z50" s="20" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="26:26" ht="15" thickBot="1">
+    <row r="51" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z51" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="26:26" ht="15" thickBot="1">
+    <row r="52" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z52" s="20" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="26:26" ht="15" thickBot="1">
+    <row r="53" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z53" s="20" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="26:26" ht="15" thickBot="1">
+    <row r="54" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z54" s="20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="26:26" ht="15" thickBot="1">
+    <row r="55" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z55" s="20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="26:26" ht="15" thickBot="1">
+    <row r="56" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z56" s="20" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="26:26" ht="15" thickBot="1">
+    <row r="57" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z57" s="20" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="26:26" ht="15" thickBot="1">
+    <row r="58" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z58" s="20" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="26:26" ht="15" thickBot="1">
+    <row r="59" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z59" s="20" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="26:26" ht="15" thickBot="1">
+    <row r="60" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z60" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="26:26" ht="15" thickBot="1">
+    <row r="61" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z61" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="26:26" ht="15" thickBot="1">
+    <row r="62" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z62" s="20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="26:26" ht="15" thickBot="1">
+    <row r="63" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z63" s="20" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="26:26" ht="15" thickBot="1">
+    <row r="64" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z64" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="26:26" ht="15" thickBot="1">
+    <row r="65" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z65" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="26:26" ht="15" thickBot="1">
+    <row r="66" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z66" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="26:26" ht="15" thickBot="1">
+    <row r="67" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z67" s="20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="68" spans="26:26" ht="15" thickBot="1">
+    <row r="68" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z68" s="20" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="69" spans="26:26" ht="15" thickBot="1">
+    <row r="69" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z69" s="20" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="26:26" ht="15" thickBot="1">
+    <row r="70" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z70" s="20" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="26:26" ht="15" thickBot="1">
+    <row r="71" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z71" s="20" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="26:26" ht="15" thickBot="1">
+    <row r="72" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z72" s="20" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="73" spans="26:26" ht="15" thickBot="1">
+    <row r="73" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z73" s="20" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="26:26" ht="15" thickBot="1">
+    <row r="74" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z74" s="20" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="26:26" ht="15" thickBot="1">
+    <row r="75" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z75" s="20" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="26:26" ht="15" thickBot="1">
+    <row r="76" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z76" s="20" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="77" spans="26:26" ht="15" thickBot="1">
+    <row r="77" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z77" s="20" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="78" spans="26:26" ht="15" thickBot="1">
+    <row r="78" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z78" s="20" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="26:26" ht="15" thickBot="1">
+    <row r="79" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z79" s="20" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="26:26" ht="15" thickBot="1">
+    <row r="80" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z80" s="20" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="81" spans="26:26" ht="15" thickBot="1">
+    <row r="81" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z81" s="20" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="82" spans="26:26" ht="15" thickBot="1">
+    <row r="82" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z82" s="20" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="83" spans="26:26" ht="15" thickBot="1">
+    <row r="83" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z83" s="20" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="84" spans="26:26" ht="15" thickBot="1">
+    <row r="84" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z84" s="20" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="85" spans="26:26" ht="15" thickBot="1">
+    <row r="85" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z85" s="20" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="86" spans="26:26" ht="15" thickBot="1">
+    <row r="86" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z86" s="20" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="87" spans="26:26" ht="15" thickBot="1">
+    <row r="87" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z87" s="20" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="26:26" ht="15" thickBot="1">
+    <row r="88" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z88" s="20" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="89" spans="26:26" ht="15" thickBot="1">
+    <row r="89" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z89" s="20" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="90" spans="26:26" ht="15" thickBot="1">
+    <row r="90" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z90" s="20" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="91" spans="26:26" ht="15" thickBot="1">
+    <row r="91" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z91" s="20" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="92" spans="26:26" ht="15" thickBot="1">
+    <row r="92" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z92" s="20" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="93" spans="26:26" ht="15" thickBot="1">
+    <row r="93" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z93" s="20" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="94" spans="26:26" ht="15" thickBot="1">
+    <row r="94" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z94" s="20" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="95" spans="26:26" ht="15" thickBot="1">
+    <row r="95" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z95" s="20" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="96" spans="26:26" ht="15" thickBot="1">
+    <row r="96" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z96" s="20" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="97" spans="26:26" ht="15" thickBot="1">
+    <row r="97" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z97" s="20" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="98" spans="26:26" ht="15" thickBot="1">
+    <row r="98" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z98" s="20" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="99" spans="26:26" ht="15" thickBot="1">
+    <row r="99" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z99" s="20" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="100" spans="26:26" ht="15" thickBot="1">
+    <row r="100" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z100" s="20" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="101" spans="26:26" ht="15" thickBot="1">
+    <row r="101" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z101" s="20" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="26:26" ht="15" thickBot="1">
+    <row r="102" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z102" s="20" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="26:26" ht="15" thickBot="1">
+    <row r="103" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z103" s="20" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="104" spans="26:26" ht="15" thickBot="1">
+    <row r="104" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z104" s="20" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="105" spans="26:26" ht="15" thickBot="1">
+    <row r="105" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z105" s="20" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="106" spans="26:26" ht="15" thickBot="1">
+    <row r="106" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z106" s="20" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="107" spans="26:26" ht="15" thickBot="1">
+    <row r="107" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z107" s="20" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="108" spans="26:26" ht="15" thickBot="1">
+    <row r="108" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z108" s="20" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="109" spans="26:26" ht="15" thickBot="1">
+    <row r="109" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z109" s="20" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="110" spans="26:26" ht="15" thickBot="1">
+    <row r="110" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z110" s="20" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="111" spans="26:26" ht="15" thickBot="1">
+    <row r="111" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z111" s="20" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="112" spans="26:26" ht="15" thickBot="1">
+    <row r="112" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z112" s="20" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="113" spans="26:26" ht="15" thickBot="1">
+    <row r="113" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z113" s="20" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="114" spans="26:26" ht="15" thickBot="1">
+    <row r="114" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z114" s="20" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="115" spans="26:26" ht="15" thickBot="1">
+    <row r="115" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z115" s="20" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="116" spans="26:26" ht="15" thickBot="1">
+    <row r="116" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z116" s="20" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="117" spans="26:26" ht="15" thickBot="1">
+    <row r="117" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z117" s="20" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="118" spans="26:26" ht="15" thickBot="1">
+    <row r="118" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z118" s="20" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="26:26" ht="15" thickBot="1">
+    <row r="119" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z119" s="20" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="120" spans="26:26" ht="15" thickBot="1">
+    <row r="120" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z120" s="20" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="121" spans="26:26" ht="15" thickBot="1">
+    <row r="121" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z121" s="20" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="122" spans="26:26" ht="15" thickBot="1">
+    <row r="122" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z122" s="20" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="123" spans="26:26" ht="15" thickBot="1">
+    <row r="123" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z123" s="20" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="124" spans="26:26" ht="15" thickBot="1">
+    <row r="124" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z124" s="20" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="125" spans="26:26" ht="15" thickBot="1">
+    <row r="125" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z125" s="20" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="126" spans="26:26" ht="15" thickBot="1">
+    <row r="126" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z126" s="20" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="127" spans="26:26" ht="15" thickBot="1">
+    <row r="127" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z127" s="20" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="128" spans="26:26" ht="15" thickBot="1">
+    <row r="128" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z128" s="20" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="26:26" ht="15" thickBot="1">
+    <row r="129" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z129" s="20" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="130" spans="26:26" ht="15" thickBot="1">
+    <row r="130" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z130" s="20" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="131" spans="26:26" ht="15" thickBot="1">
+    <row r="131" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z131" s="20" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="132" spans="26:26" ht="15" thickBot="1">
+    <row r="132" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z132" s="20" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="133" spans="26:26" ht="15" thickBot="1">
+    <row r="133" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z133" s="20" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="134" spans="26:26" ht="15" thickBot="1">
+    <row r="134" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z134" s="20" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="135" spans="26:26" ht="15" thickBot="1">
+    <row r="135" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z135" s="20" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="136" spans="26:26" ht="15" thickBot="1">
+    <row r="136" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z136" s="20" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="137" spans="26:26" ht="15" thickBot="1">
+    <row r="137" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z137" s="20" t="s">
         <v>186</v>
       </c>
@@ -2310,13 +2496,13 @@
       <selection activeCell="F2" sqref="F2:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2483,4 +2669,388 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="P1" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q1" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="S1" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="T1" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="U1" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="V1" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="W1" s="24" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" t="s">
+        <v>258</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="G4" s="27">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="G5" s="27">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="D6" t="s">
+        <v>258</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="I6" s="27">
+        <v>1</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="M6" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" t="s">
+        <v>258</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" t="s">
+        <v>258</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="27"/>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="I9" s="27">
+        <v>1</v>
+      </c>
+      <c r="J9" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="K9" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" t="s">
+        <v>258</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="I10" s="27">
+        <v>1</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="M10" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="D11" t="s">
+        <v>258</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="I11" s="27">
+        <v>1</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="L11" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="M11" s="27">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
voice call issue fix
</commit_message>
<xml_diff>
--- a/Input_sheet_V2.xlsx
+++ b/Input_sheet_V2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="234">
   <si>
     <t>Execution</t>
   </si>
@@ -662,58 +662,61 @@
     <t>device2</t>
   </si>
   <si>
-    <t>Du-National calls: VOICE_NAT</t>
-  </si>
-  <si>
-    <t>Du-National calls: VOICE_NAT_OFF</t>
-  </si>
-  <si>
-    <t>Du-National calls: VOICE_NAT_WK</t>
-  </si>
-  <si>
-    <t>Du-National calls: VOICE_NAT_OFF_WK</t>
-  </si>
-  <si>
-    <t>Du-International calls: VOICE_INT_IDD</t>
-  </si>
-  <si>
-    <t>Du-International calls: VOICE_INT_IDD_OFF</t>
-  </si>
-  <si>
-    <t>Du-International calls: VOICE_INT_IDD_WK</t>
-  </si>
-  <si>
-    <t>Du-International calls: VOICE_INT_IDD_OFF_WK</t>
-  </si>
-  <si>
     <t>Du-du calls: VOICE_DU</t>
   </si>
   <si>
-    <t>Du-du calls: VOICE_DU_OFF</t>
-  </si>
-  <si>
-    <t>Du-du calls: VOICE_DU_WK</t>
-  </si>
-  <si>
-    <t>Du-du calls: VOICE_DU_OFF_WK</t>
-  </si>
-  <si>
-    <t>Du-CUG calls: VOICE_DU_CUG</t>
-  </si>
-  <si>
-    <t>Du-CUG calls: VOICE_DU_OFF_CUG</t>
-  </si>
-  <si>
-    <t>Du-CUG calls: VOICE_DU_WK_CUG</t>
-  </si>
-  <si>
-    <t>Du-CUG calls: VOICE_DU_OFF_WK_CUG</t>
-  </si>
-  <si>
-    <t>Roaming calls: VOICE_INT_ROAM</t>
-  </si>
-  <si>
     <t>TC_009</t>
+  </si>
+  <si>
+    <t>Du-du calls_VOICE_DU</t>
+  </si>
+  <si>
+    <t>Du-du calls_VOICE_DU_OFF</t>
+  </si>
+  <si>
+    <t>Du-du calls_VOICE_DU_WK</t>
+  </si>
+  <si>
+    <t>Du-du calls_VOICE_DU_OFF_WK</t>
+  </si>
+  <si>
+    <t>Du-CUG calls_VOICE_DU_CUG</t>
+  </si>
+  <si>
+    <t>Du-CUG calls_VOICE_DU_OFF_CUG</t>
+  </si>
+  <si>
+    <t>Du-CUG calls_VOICE_DU_WK_CUG</t>
+  </si>
+  <si>
+    <t>Du-CUG calls_VOICE_DU_OFF_WK_CUG</t>
+  </si>
+  <si>
+    <t>Roaming calls_VOICE_INT_ROAM</t>
+  </si>
+  <si>
+    <t>Du-National calls_VOICE_NAT</t>
+  </si>
+  <si>
+    <t>Du-National calls_VOICE_NAT_OFF</t>
+  </si>
+  <si>
+    <t>Du-National calls_VOICE_NAT_WK</t>
+  </si>
+  <si>
+    <t>Du-National calls_VOICE_NAT_OFF_WK</t>
+  </si>
+  <si>
+    <t>Du-International calls_VOICE_INT_IDD</t>
+  </si>
+  <si>
+    <t>Du-International calls_VOICE_INT_IDD_OFF</t>
+  </si>
+  <si>
+    <t>Du-International calls_VOICE_INT_IDD_WK</t>
+  </si>
+  <si>
+    <t>Du-International calls_VOICE_INT_IDD_OFF_WK</t>
   </si>
 </sst>
 </file>
@@ -1211,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Z1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1232,11 +1235,12 @@
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.453125" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="26.1796875" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="17.54296875" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="41.7265625" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="41.26953125" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="15.7265625" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="19.90625" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="15.7265625" hidden="1" customWidth="1"/>
@@ -1431,7 +1435,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>39</v>
@@ -1646,7 +1650,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>43</v>
@@ -1709,7 +1713,7 @@
     </row>
     <row r="15" spans="1:26">
       <c r="U15" s="24" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="Z15" s="17" t="s">
         <v>60</v>
@@ -1717,7 +1721,7 @@
     </row>
     <row r="16" spans="1:26">
       <c r="U16" s="24" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="Z16" s="17" t="s">
         <v>61</v>
@@ -1725,7 +1729,7 @@
     </row>
     <row r="17" spans="21:26">
       <c r="U17" s="24" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="Z17" s="17" t="s">
         <v>62</v>
@@ -1733,7 +1737,7 @@
     </row>
     <row r="18" spans="21:26" ht="15" thickBot="1">
       <c r="U18" s="24" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="Z18" s="17" t="s">
         <v>63</v>
@@ -1741,7 +1745,7 @@
     </row>
     <row r="19" spans="21:26" ht="15" thickBot="1">
       <c r="U19" s="24" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="Z19" s="18" t="s">
         <v>64</v>
@@ -1749,7 +1753,7 @@
     </row>
     <row r="20" spans="21:26" ht="15" thickBot="1">
       <c r="U20" s="24" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="Z20" s="19" t="s">
         <v>65</v>
@@ -1757,7 +1761,7 @@
     </row>
     <row r="21" spans="21:26" ht="15" thickBot="1">
       <c r="U21" s="24" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="Z21" s="19" t="s">
         <v>66</v>
@@ -1765,7 +1769,7 @@
     </row>
     <row r="22" spans="21:26" ht="15" thickBot="1">
       <c r="U22" s="25" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="Z22" s="19" t="s">
         <v>67</v>
@@ -1773,7 +1777,7 @@
     </row>
     <row r="23" spans="21:26" ht="15" thickBot="1">
       <c r="U23" s="24" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="Z23" s="19" t="s">
         <v>68</v>
@@ -1781,7 +1785,7 @@
     </row>
     <row r="24" spans="21:26" ht="15" thickBot="1">
       <c r="U24" s="24" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="Z24" s="19" t="s">
         <v>69</v>
@@ -1789,7 +1793,7 @@
     </row>
     <row r="25" spans="21:26" ht="15" thickBot="1">
       <c r="U25" s="24" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="Z25" s="19" t="s">
         <v>70</v>
@@ -1797,7 +1801,7 @@
     </row>
     <row r="26" spans="21:26" ht="15" thickBot="1">
       <c r="U26" s="24" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="Z26" s="20" t="s">
         <v>71</v>
@@ -1805,7 +1809,7 @@
     </row>
     <row r="27" spans="21:26" ht="15" thickBot="1">
       <c r="U27" s="24" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="Z27" s="20" t="s">
         <v>72</v>
@@ -1813,7 +1817,7 @@
     </row>
     <row r="28" spans="21:26" ht="15" thickBot="1">
       <c r="U28" s="24" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="Z28" s="20" t="s">
         <v>73</v>
@@ -1821,7 +1825,7 @@
     </row>
     <row r="29" spans="21:26" ht="15" thickBot="1">
       <c r="U29" s="24" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="Z29" s="20" t="s">
         <v>74</v>
@@ -1829,7 +1833,7 @@
     </row>
     <row r="30" spans="21:26" ht="15" thickBot="1">
       <c r="U30" s="24" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="Z30" s="20" t="s">
         <v>75</v>
@@ -1837,7 +1841,7 @@
     </row>
     <row r="31" spans="21:26" ht="15" thickBot="1">
       <c r="U31" s="24" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="Z31" s="20" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
API integ with result
</commit_message>
<xml_diff>
--- a/Input_sheet_V2.xlsx
+++ b/Input_sheet_V2.xlsx
@@ -838,7 +838,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,8 +898,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -927,12 +934,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1005,7 +1006,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1047,10 +1048,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2670,10 +2673,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2693,10 +2696,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="22" t="s">
         <v>225</v>
       </c>
       <c r="C1" s="24" t="s">
@@ -2764,10 +2767,10 @@
       </c>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -2779,12 +2782,14 @@
       <c r="E2" s="11" t="s">
         <v>46</v>
       </c>
+      <c r="G2" s="29"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:23">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="22" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -2796,12 +2801,14 @@
       <c r="E3" s="11" t="s">
         <v>46</v>
       </c>
+      <c r="G3" s="29"/>
+      <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -2813,18 +2820,19 @@
       <c r="E4" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="25" t="s">
         <v>258</v>
       </c>
       <c r="G4" s="27">
         <v>1001</v>
       </c>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -2836,18 +2844,19 @@
       <c r="E5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="25" t="s">
         <v>258</v>
       </c>
       <c r="G5" s="27">
         <v>351</v>
       </c>
+      <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="22" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -2859,25 +2868,25 @@
       <c r="E6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="25" t="s">
         <v>259</v>
       </c>
       <c r="G6" s="27" t="s">
         <v>260</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="25" t="s">
         <v>261</v>
       </c>
       <c r="I6" s="27">
         <v>1</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="K6" s="28" t="s">
+      <c r="K6" s="30" t="s">
         <v>263</v>
       </c>
-      <c r="L6" s="26" t="s">
+      <c r="L6" s="25" t="s">
         <v>264</v>
       </c>
       <c r="M6" s="27">
@@ -2885,10 +2894,10 @@
       </c>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -2900,18 +2909,19 @@
       <c r="E7" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="28" t="s">
         <v>265</v>
       </c>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -2923,18 +2933,18 @@
       <c r="E8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="22" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -2946,19 +2956,19 @@
       <c r="E9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="28" t="s">
         <v>267</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="28">
         <v>1</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="25" t="s">
         <v>269</v>
       </c>
       <c r="K9" s="27">
@@ -2966,10 +2976,10 @@
       </c>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="22" t="s">
         <v>226</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -2981,25 +2991,25 @@
       <c r="E10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="25" t="s">
         <v>259</v>
       </c>
       <c r="G10" s="27" t="s">
         <v>260</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="H10" s="25" t="s">
         <v>261</v>
       </c>
       <c r="I10" s="27">
         <v>1</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="K10" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="L10" s="26" t="s">
+      <c r="L10" s="25" t="s">
         <v>264</v>
       </c>
       <c r="M10" s="27">
@@ -3007,47 +3017,904 @@
       </c>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="22" t="s">
         <v>227</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="22" t="s">
         <v>257</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="25" t="s">
         <v>261</v>
       </c>
       <c r="I11" s="27">
         <v>1</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="K11" s="28" t="s">
+      <c r="K11" s="30" t="s">
         <v>263</v>
       </c>
-      <c r="L11" s="26" t="s">
+      <c r="L11" s="25" t="s">
         <v>264</v>
       </c>
       <c r="M11" s="27">
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="1:23">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="27"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="27"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="27"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="27"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="27"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="27"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="27"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="27"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="30"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="27"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="22"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="22"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
+      <c r="M43" s="22"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="22"/>
+      <c r="M45" s="22"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="25"/>
+      <c r="M46" s="27"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="22"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="22"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="22"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="25"/>
+      <c r="K48" s="26"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="22"/>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="22"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="25"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="22"/>
+      <c r="M49" s="22"/>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="25"/>
+      <c r="K50" s="30"/>
+      <c r="L50" s="25"/>
+      <c r="M50" s="27"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="22"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="27"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="25"/>
+      <c r="M51" s="27"/>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="22"/>
+      <c r="B52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="22"/>
+      <c r="B53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="22"/>
+      <c r="B54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="22"/>
+      <c r="B55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="22"/>
+      <c r="B56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="22"/>
+      <c r="B57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="22"/>
+      <c r="B58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="22"/>
+      <c r="B59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="22"/>
+      <c r="B60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="22"/>
+      <c r="B61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" s="22"/>
+      <c r="B62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="22"/>
+      <c r="B64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="22"/>
+      <c r="B65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="22"/>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="22"/>
+      <c r="G68" s="22"/>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="22"/>
+      <c r="G73" s="22"/>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="D75" s="22"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="22"/>
+      <c r="G75" s="22"/>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="22"/>
+      <c r="G76" s="22"/>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="D77" s="22"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="22"/>
+      <c r="G77" s="22"/>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="22"/>
+      <c r="G78" s="22"/>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="22"/>
+    </row>
+    <row r="81" spans="4:7">
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="22"/>
+    </row>
+    <row r="82" spans="4:7">
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
+    </row>
+    <row r="83" spans="4:7">
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="22"/>
+    </row>
+    <row r="84" spans="4:7">
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="22"/>
+      <c r="G84" s="22"/>
+    </row>
+    <row r="85" spans="4:7">
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="22"/>
+    </row>
+    <row r="86" spans="4:7">
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
+      <c r="G86" s="22"/>
+    </row>
+    <row r="87" spans="4:7">
+      <c r="D87" s="22"/>
+      <c r="E87" s="22"/>
+      <c r="F87" s="22"/>
+      <c r="G87" s="22"/>
+    </row>
+    <row r="88" spans="4:7">
+      <c r="D88" s="22"/>
+      <c r="E88" s="22"/>
+      <c r="F88" s="22"/>
+      <c r="G88" s="22"/>
+    </row>
+    <row r="89" spans="4:7">
+      <c r="D89" s="22"/>
+      <c r="E89" s="22"/>
+      <c r="F89" s="22"/>
+      <c r="G89" s="22"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes after string tag
</commit_message>
<xml_diff>
--- a/Input_sheet_V2.xlsx
+++ b/Input_sheet_V2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="273">
   <si>
     <t>Execution</t>
   </si>
@@ -832,6 +832,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -2676,7 +2679,7 @@
   <dimension ref="A1:W89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A3" sqref="A3:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2787,7 +2790,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>6</v>
@@ -2806,7 +2809,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>7</v>
@@ -2830,7 +2833,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>8</v>
@@ -2848,13 +2851,13 @@
         <v>258</v>
       </c>
       <c r="G5" s="27">
-        <v>351</v>
+        <v>1001</v>
       </c>
       <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>9</v>
@@ -2895,7 +2898,7 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" s="22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>11</v>
@@ -2919,7 +2922,7 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>13</v>
@@ -2942,7 +2945,7 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" s="22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>15</v>
@@ -2977,7 +2980,7 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>226</v>
@@ -3018,7 +3021,7 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>227</v>

</xml_diff>

<commit_message>
dual sim sms handled
</commit_message>
<xml_diff>
--- a/Input_sheet_V2.xlsx
+++ b/Input_sheet_V2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="280">
   <si>
     <t>Execution</t>
   </si>
@@ -767,21 +767,6 @@
     <t>Rework_65</t>
   </si>
   <si>
-    <t>MSISDN Moredata20</t>
-  </si>
-  <si>
-    <t>MSISDN Moredata50</t>
-  </si>
-  <si>
-    <t>MSISDN Moredata100</t>
-  </si>
-  <si>
-    <t>MSISDN Moredata200</t>
-  </si>
-  <si>
-    <t>MSISDN Moredata500</t>
-  </si>
-  <si>
     <t>Kabayan  ChatnCall  Recurrent  daily bundle</t>
   </si>
   <si>
@@ -843,6 +828,33 @@
   </si>
   <si>
     <t>971520002574</t>
+  </si>
+  <si>
+    <t>Rework_60</t>
+  </si>
+  <si>
+    <t>Rework_61</t>
+  </si>
+  <si>
+    <t>Rework_62</t>
+  </si>
+  <si>
+    <t>9732</t>
+  </si>
+  <si>
+    <t>971520001714 Moredata20</t>
+  </si>
+  <si>
+    <t>971520001714 Moredata50</t>
+  </si>
+  <si>
+    <t>971520001714 Moredata100</t>
+  </si>
+  <si>
+    <t>971520001714 Moredata200</t>
+  </si>
+  <si>
+    <t>971520001714 Moredata500</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1448,7 @@
   <dimension ref="A1:Z185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1519,7 +1531,7 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>235</v>
@@ -1604,7 +1616,7 @@
     </row>
     <row r="4" spans="1:26" s="22" customFormat="1">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>238</v>
@@ -1727,7 +1739,7 @@
     </row>
     <row r="7" spans="1:26" s="22" customFormat="1">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>239</v>
@@ -1765,7 +1777,7 @@
     </row>
     <row r="8" spans="1:26" s="35" customFormat="1">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="31" t="s">
         <v>240</v>
@@ -1774,7 +1786,7 @@
         <v>42</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>18</v>
+        <v>246</v>
       </c>
       <c r="E8" s="31" t="s">
         <v>23</v>
@@ -1787,10 +1799,10 @@
       <c r="I8" s="33"/>
       <c r="J8" s="34"/>
       <c r="K8" s="32" t="s">
-        <v>49</v>
+        <v>274</v>
       </c>
       <c r="L8" s="31" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="M8" s="31">
         <v>1</v>
@@ -1831,7 +1843,7 @@
         <v>42</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>18</v>
+        <v>246</v>
       </c>
       <c r="E9" s="31" t="s">
         <v>23</v>
@@ -1844,10 +1856,10 @@
       <c r="I9" s="33"/>
       <c r="J9" s="34"/>
       <c r="K9" s="32" t="s">
-        <v>49</v>
+        <v>274</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>251</v>
+        <v>276</v>
       </c>
       <c r="M9" s="31">
         <v>1</v>
@@ -1882,13 +1894,13 @@
         <v>30</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>240</v>
+        <v>271</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>18</v>
+        <v>246</v>
       </c>
       <c r="E10" s="31" t="s">
         <v>23</v>
@@ -1901,10 +1913,10 @@
       <c r="I10" s="33"/>
       <c r="J10" s="34"/>
       <c r="K10" s="32" t="s">
-        <v>49</v>
+        <v>274</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="M10" s="31">
         <v>1</v>
@@ -1939,13 +1951,13 @@
         <v>30</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>241</v>
+        <v>272</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>18</v>
+        <v>246</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>23</v>
@@ -1958,10 +1970,10 @@
       <c r="I11" s="33"/>
       <c r="J11" s="34"/>
       <c r="K11" s="32" t="s">
-        <v>49</v>
+        <v>274</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>253</v>
+        <v>278</v>
       </c>
       <c r="M11" s="31">
         <v>1</v>
@@ -1996,13 +2008,13 @@
         <v>30</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>241</v>
+        <v>273</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>18</v>
+        <v>246</v>
       </c>
       <c r="E12" s="31" t="s">
         <v>23</v>
@@ -2015,10 +2027,10 @@
       <c r="I12" s="33"/>
       <c r="J12" s="34"/>
       <c r="K12" s="32" t="s">
-        <v>49</v>
+        <v>274</v>
       </c>
       <c r="L12" s="31" t="s">
-        <v>254</v>
+        <v>279</v>
       </c>
       <c r="M12" s="31">
         <v>1</v>
@@ -2050,7 +2062,7 @@
     </row>
     <row r="13" spans="1:26" s="30" customFormat="1">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="26" t="s">
         <v>247</v>
@@ -2135,7 +2147,7 @@
     </row>
     <row r="15" spans="1:26" s="30" customFormat="1">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>248</v>
@@ -2220,7 +2232,7 @@
     </row>
     <row r="17" spans="1:26" s="30" customFormat="1">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>249</v>
@@ -2305,10 +2317,10 @@
     </row>
     <row r="19" spans="1:26" s="30" customFormat="1">
       <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>42</v>
@@ -2323,7 +2335,7 @@
         <v>38</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
@@ -2339,7 +2351,7 @@
         <v>30</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>42</v>
@@ -2391,10 +2403,10 @@
     </row>
     <row r="21" spans="1:26" s="30" customFormat="1">
       <c r="A21" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>42</v>
@@ -2409,7 +2421,7 @@
         <v>38</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
@@ -2422,10 +2434,10 @@
     </row>
     <row r="22" spans="1:26" s="30" customFormat="1">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>42</v>
@@ -2440,7 +2452,7 @@
         <v>38</v>
       </c>
       <c r="G22" s="26" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
@@ -2456,7 +2468,7 @@
         <v>30</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>42</v>
@@ -2489,10 +2501,10 @@
     </row>
     <row r="24" spans="1:26" s="30" customFormat="1">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>42</v>
@@ -2507,7 +2519,7 @@
         <v>38</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
@@ -2520,10 +2532,10 @@
     </row>
     <row r="25" spans="1:26" s="30" customFormat="1">
       <c r="A25" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>42</v>
@@ -2554,7 +2566,7 @@
         <v>30</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>42</v>
@@ -2587,10 +2599,10 @@
     </row>
     <row r="27" spans="1:26" s="30" customFormat="1">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>42</v>
@@ -2617,11 +2629,11 @@
       <c r="O27" s="27"/>
     </row>
     <row r="28" spans="1:26" s="30" customFormat="1">
-      <c r="A28" s="26" t="s">
-        <v>29</v>
+      <c r="A28" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>42</v>
@@ -2636,7 +2648,7 @@
         <v>38</v>
       </c>
       <c r="G28" s="26" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
@@ -2648,11 +2660,11 @@
       <c r="O28" s="27"/>
     </row>
     <row r="29" spans="1:26" s="30" customFormat="1">
-      <c r="A29" s="26" t="s">
-        <v>29</v>
+      <c r="A29" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>42</v>
@@ -2667,7 +2679,7 @@
         <v>38</v>
       </c>
       <c r="G29" s="26" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
@@ -2679,11 +2691,11 @@
       <c r="O29" s="27"/>
     </row>
     <row r="30" spans="1:26" s="30" customFormat="1">
-      <c r="A30" s="26" t="s">
-        <v>29</v>
+      <c r="A30" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>42</v>
@@ -2698,7 +2710,7 @@
         <v>38</v>
       </c>
       <c r="G30" s="26" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>
@@ -2710,11 +2722,11 @@
       <c r="O30" s="27"/>
     </row>
     <row r="31" spans="1:26" s="30" customFormat="1">
-      <c r="A31" s="26" t="s">
-        <v>29</v>
+      <c r="A31" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>42</v>
@@ -2729,7 +2741,7 @@
         <v>38</v>
       </c>
       <c r="G31" s="26" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
@@ -2741,11 +2753,11 @@
       <c r="O31" s="27"/>
     </row>
     <row r="32" spans="1:26" s="30" customFormat="1">
-      <c r="A32" s="26" t="s">
-        <v>29</v>
+      <c r="A32" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>42</v>
@@ -2760,7 +2772,7 @@
         <v>38</v>
       </c>
       <c r="G32" s="26" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H32" s="28"/>
       <c r="I32" s="28"/>
@@ -2772,11 +2784,11 @@
       <c r="O32" s="27"/>
     </row>
     <row r="33" spans="1:26" s="30" customFormat="1">
-      <c r="A33" s="26" t="s">
-        <v>29</v>
+      <c r="A33" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>42</v>
@@ -2791,7 +2803,7 @@
         <v>38</v>
       </c>
       <c r="G33" s="26" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
@@ -2803,11 +2815,11 @@
       <c r="O33" s="27"/>
     </row>
     <row r="34" spans="1:26" s="30" customFormat="1">
-      <c r="A34" s="26" t="s">
-        <v>29</v>
+      <c r="A34" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C34" s="26" t="s">
         <v>42</v>
@@ -2822,7 +2834,7 @@
         <v>38</v>
       </c>
       <c r="G34" s="26" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
@@ -2834,11 +2846,11 @@
       <c r="O34" s="27"/>
     </row>
     <row r="35" spans="1:26" s="30" customFormat="1">
-      <c r="A35" s="26" t="s">
-        <v>29</v>
+      <c r="A35" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C35" s="26" t="s">
         <v>42</v>
@@ -2853,7 +2865,7 @@
         <v>38</v>
       </c>
       <c r="G35" s="26" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="H35" s="28"/>
       <c r="I35" s="28"/>
@@ -2865,11 +2877,11 @@
       <c r="O35" s="27"/>
     </row>
     <row r="36" spans="1:26" s="30" customFormat="1">
-      <c r="A36" s="26" t="s">
-        <v>29</v>
+      <c r="A36" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C36" s="26" t="s">
         <v>42</v>
@@ -2896,11 +2908,11 @@
       <c r="O36" s="27"/>
     </row>
     <row r="37" spans="1:26" s="30" customFormat="1">
-      <c r="A37" s="26" t="s">
-        <v>29</v>
+      <c r="A37" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C37" s="26" t="s">
         <v>42</v>
@@ -2927,11 +2939,11 @@
       <c r="O37" s="27"/>
     </row>
     <row r="38" spans="1:26" s="30" customFormat="1">
-      <c r="A38" s="26" t="s">
-        <v>29</v>
+      <c r="A38" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C38" s="26" t="s">
         <v>42</v>
@@ -2943,10 +2955,10 @@
         <v>46</v>
       </c>
       <c r="F38" s="27" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="H38" s="28"/>
       <c r="I38" s="28"/>
@@ -2958,11 +2970,11 @@
       <c r="O38" s="27"/>
     </row>
     <row r="39" spans="1:26" s="30" customFormat="1">
-      <c r="A39" s="26" t="s">
-        <v>29</v>
+      <c r="A39" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C39" s="26" t="s">
         <v>42</v>
@@ -2974,10 +2986,10 @@
         <v>46</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G39" s="26" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="H39" s="28"/>
       <c r="I39" s="28"/>
@@ -4066,37 +4078,37 @@
     </row>
     <row r="179" spans="26:26">
       <c r="Z179" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="180" spans="26:26">
       <c r="Z180" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="181" spans="26:26">
       <c r="Z181" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="182" spans="26:26">
       <c r="Z182" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="183" spans="26:26">
       <c r="Z183" s="22" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="184" spans="26:26">
       <c r="Z184" s="22" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="185" spans="26:26">
       <c r="Z185" s="46" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -4136,7 +4148,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F2" sqref="F2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4185,7 +4197,7 @@
         <v>212</v>
       </c>
       <c r="F2" s="22">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -4205,7 +4217,7 @@
         <v>194</v>
       </c>
       <c r="F3" s="22">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -4225,7 +4237,7 @@
         <v>197</v>
       </c>
       <c r="F4" s="22">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -4245,7 +4257,7 @@
         <v>197</v>
       </c>
       <c r="F5" s="22">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -4265,7 +4277,7 @@
         <v>202</v>
       </c>
       <c r="F6" s="22">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4285,7 +4297,7 @@
         <v>206</v>
       </c>
       <c r="F7" s="22">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -4305,7 +4317,7 @@
         <v>208</v>
       </c>
       <c r="F8" s="22">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final commit GUI base
</commit_message>
<xml_diff>
--- a/Input_sheet_V2.xlsx
+++ b/Input_sheet_V2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Execution_Sheet" sheetId="5" r:id="rId1"/>
@@ -666,7 +666,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -1156,36 +1156,36 @@
   <dimension ref="A1:Z138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.90625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.90625" customWidth="1"/>
-    <col min="11" max="11" width="16.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="26.1796875" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="17.54296875" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="27.90625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7265625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="19.90625" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="15.7265625" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="15.54296875" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="38.453125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="26.140625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="27.85546875" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="19.85546875" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="38.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="5" customFormat="1">
@@ -1238,7 +1238,7 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
@@ -1659,602 +1659,602 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="26:26" ht="15" thickBot="1">
+    <row r="19" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z19" s="20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="26:26" ht="15" thickBot="1">
+    <row r="20" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z20" s="21" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="26:26" ht="15" thickBot="1">
+    <row r="21" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z21" s="22" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="26:26" ht="15" thickBot="1">
+    <row r="22" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z22" s="22" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="26:26" ht="15" thickBot="1">
+    <row r="23" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z23" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="26:26" ht="15" thickBot="1">
+    <row r="24" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z24" s="22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="26:26" ht="15" thickBot="1">
+    <row r="25" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z25" s="22" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="26:26" ht="15" thickBot="1">
+    <row r="26" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z26" s="22" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="26:26" ht="15" thickBot="1">
+    <row r="27" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z27" s="23" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="26:26" ht="15" thickBot="1">
+    <row r="28" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z28" s="23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="26:26" ht="15" thickBot="1">
+    <row r="29" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z29" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="26:26" ht="15" thickBot="1">
+    <row r="30" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z30" s="23" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="26:26" ht="15" thickBot="1">
+    <row r="31" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z31" s="23" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="26:26" ht="15" thickBot="1">
+    <row r="32" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z32" s="23" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="26:26" ht="15" thickBot="1">
+    <row r="33" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z33" s="23" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="26:26" ht="15" thickBot="1">
+    <row r="34" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z34" s="23" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="26:26" ht="15" thickBot="1">
+    <row r="35" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z35" s="23" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="26:26" ht="15" thickBot="1">
+    <row r="36" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z36" s="23" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="26:26" ht="15" thickBot="1">
+    <row r="37" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z37" s="23" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="26:26" ht="15" thickBot="1">
+    <row r="38" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z38" s="23" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="26:26" ht="15" thickBot="1">
+    <row r="39" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z39" s="23" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="26:26" ht="15" thickBot="1">
+    <row r="40" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z40" s="23" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="26:26" ht="15" thickBot="1">
+    <row r="41" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z41" s="23" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="26:26" ht="15" thickBot="1">
+    <row r="42" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z42" s="23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="26:26" ht="15" thickBot="1">
+    <row r="43" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z43" s="23" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="26:26" ht="15" thickBot="1">
+    <row r="44" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z44" s="23" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="26:26" ht="15" thickBot="1">
+    <row r="45" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z45" s="23" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="26:26" ht="15" thickBot="1">
+    <row r="46" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z46" s="23" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="26:26" ht="15" thickBot="1">
+    <row r="47" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z47" s="23" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="26:26" ht="15" thickBot="1">
+    <row r="48" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z48" s="23" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="26:26" ht="15" thickBot="1">
+    <row r="49" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z49" s="23" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="26:26" ht="15" thickBot="1">
+    <row r="50" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z50" s="23" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="26:26" ht="15" thickBot="1">
+    <row r="51" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z51" s="23" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="26:26" ht="15" thickBot="1">
+    <row r="52" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z52" s="23" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="26:26" ht="15" thickBot="1">
+    <row r="53" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z53" s="23" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="26:26" ht="15" thickBot="1">
+    <row r="54" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z54" s="23" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="26:26" ht="15" thickBot="1">
+    <row r="55" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z55" s="23" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="26:26" ht="15" thickBot="1">
+    <row r="56" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z56" s="23" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="26:26" ht="15" thickBot="1">
+    <row r="57" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z57" s="23" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="26:26" ht="15" thickBot="1">
+    <row r="58" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z58" s="23" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="26:26" ht="15" thickBot="1">
+    <row r="59" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z59" s="23" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="26:26" ht="15" thickBot="1">
+    <row r="60" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z60" s="23" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="26:26" ht="15" thickBot="1">
+    <row r="61" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z61" s="23" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="26:26" ht="15" thickBot="1">
+    <row r="62" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z62" s="23" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="26:26" ht="15" thickBot="1">
+    <row r="63" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z63" s="23" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="26:26" ht="15" thickBot="1">
+    <row r="64" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z64" s="23" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="26:26" ht="15" thickBot="1">
+    <row r="65" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z65" s="23" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="66" spans="26:26" ht="15" thickBot="1">
+    <row r="66" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z66" s="23" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="26:26" ht="15" thickBot="1">
+    <row r="67" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z67" s="23" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="26:26" ht="15" thickBot="1">
+    <row r="68" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z68" s="23" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="26:26" ht="15" thickBot="1">
+    <row r="69" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z69" s="23" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="26:26" ht="15" thickBot="1">
+    <row r="70" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z70" s="23" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="26:26" ht="15" thickBot="1">
+    <row r="71" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z71" s="23" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="26:26" ht="15" thickBot="1">
+    <row r="72" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z72" s="23" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="26:26" ht="15" thickBot="1">
+    <row r="73" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z73" s="23" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="74" spans="26:26" ht="15" thickBot="1">
+    <row r="74" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z74" s="23" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="75" spans="26:26" ht="15" thickBot="1">
+    <row r="75" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z75" s="23" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="26:26" ht="15" thickBot="1">
+    <row r="76" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z76" s="23" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="26:26" ht="15" thickBot="1">
+    <row r="77" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z77" s="23" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="78" spans="26:26" ht="15" thickBot="1">
+    <row r="78" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z78" s="23" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="26:26" ht="15" thickBot="1">
+    <row r="79" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z79" s="23" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="80" spans="26:26" ht="15" thickBot="1">
+    <row r="80" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z80" s="23" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="26:26" ht="15" thickBot="1">
+    <row r="81" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z81" s="23" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="82" spans="26:26" ht="15" thickBot="1">
+    <row r="82" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z82" s="23" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="83" spans="26:26" ht="15" thickBot="1">
+    <row r="83" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z83" s="23" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="84" spans="26:26" ht="15" thickBot="1">
+    <row r="84" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z84" s="23" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="85" spans="26:26" ht="15" thickBot="1">
+    <row r="85" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z85" s="23" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="86" spans="26:26" ht="15" thickBot="1">
+    <row r="86" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z86" s="23" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="87" spans="26:26" ht="15" thickBot="1">
+    <row r="87" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z87" s="23" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="88" spans="26:26" ht="15" thickBot="1">
+    <row r="88" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z88" s="23" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="89" spans="26:26" ht="15" thickBot="1">
+    <row r="89" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z89" s="23" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="90" spans="26:26" ht="15" thickBot="1">
+    <row r="90" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z90" s="23" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="91" spans="26:26" ht="15" thickBot="1">
+    <row r="91" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z91" s="23" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="92" spans="26:26" ht="15" thickBot="1">
+    <row r="92" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z92" s="23" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="93" spans="26:26" ht="15" thickBot="1">
+    <row r="93" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z93" s="23" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="94" spans="26:26" ht="15" thickBot="1">
+    <row r="94" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z94" s="23" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="95" spans="26:26" ht="15" thickBot="1">
+    <row r="95" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z95" s="23" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="96" spans="26:26" ht="15" thickBot="1">
+    <row r="96" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z96" s="23" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="97" spans="26:26" ht="15" thickBot="1">
+    <row r="97" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z97" s="23" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="98" spans="26:26" ht="15" thickBot="1">
+    <row r="98" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z98" s="23" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="99" spans="26:26" ht="15" thickBot="1">
+    <row r="99" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z99" s="23" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="100" spans="26:26" ht="15" thickBot="1">
+    <row r="100" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z100" s="23" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="101" spans="26:26" ht="15" thickBot="1">
+    <row r="101" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z101" s="23" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="102" spans="26:26" ht="15" thickBot="1">
+    <row r="102" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z102" s="23" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="103" spans="26:26" ht="15" thickBot="1">
+    <row r="103" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z103" s="23" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="104" spans="26:26" ht="15" thickBot="1">
+    <row r="104" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z104" s="23" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="105" spans="26:26" ht="15" thickBot="1">
+    <row r="105" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z105" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="106" spans="26:26" ht="15" thickBot="1">
+    <row r="106" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z106" s="23" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="107" spans="26:26" ht="15" thickBot="1">
+    <row r="107" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z107" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="108" spans="26:26" ht="15" thickBot="1">
+    <row r="108" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z108" s="23" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="109" spans="26:26" ht="15" thickBot="1">
+    <row r="109" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z109" s="23" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="110" spans="26:26" ht="15" thickBot="1">
+    <row r="110" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z110" s="23" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="111" spans="26:26" ht="15" thickBot="1">
+    <row r="111" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z111" s="23" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="112" spans="26:26" ht="15" thickBot="1">
+    <row r="112" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z112" s="23" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="113" spans="26:26" ht="15" thickBot="1">
+    <row r="113" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z113" s="23" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="114" spans="26:26" ht="15" thickBot="1">
+    <row r="114" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z114" s="23" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="115" spans="26:26" ht="15" thickBot="1">
+    <row r="115" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z115" s="23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="116" spans="26:26" ht="15" thickBot="1">
+    <row r="116" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z116" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="117" spans="26:26" ht="15" thickBot="1">
+    <row r="117" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z117" s="23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="118" spans="26:26" ht="15" thickBot="1">
+    <row r="118" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z118" s="23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="119" spans="26:26" ht="15" thickBot="1">
+    <row r="119" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z119" s="23" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="120" spans="26:26" ht="15" thickBot="1">
+    <row r="120" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z120" s="23" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="121" spans="26:26" ht="15" thickBot="1">
+    <row r="121" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z121" s="23" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="122" spans="26:26" ht="15" thickBot="1">
+    <row r="122" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z122" s="23" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="123" spans="26:26" ht="15" thickBot="1">
+    <row r="123" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z123" s="23" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="124" spans="26:26" ht="15" thickBot="1">
+    <row r="124" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z124" s="23" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="125" spans="26:26" ht="15" thickBot="1">
+    <row r="125" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z125" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="126" spans="26:26" ht="15" thickBot="1">
+    <row r="126" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z126" s="23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="127" spans="26:26" ht="15" thickBot="1">
+    <row r="127" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z127" s="23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="128" spans="26:26" ht="15" thickBot="1">
+    <row r="128" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z128" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="129" spans="26:26" ht="15" thickBot="1">
+    <row r="129" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z129" s="23" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="130" spans="26:26" ht="15" thickBot="1">
+    <row r="130" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z130" s="23" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="131" spans="26:26" ht="15" thickBot="1">
+    <row r="131" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z131" s="23" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="132" spans="26:26" ht="15" thickBot="1">
+    <row r="132" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z132" s="23" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="133" spans="26:26" ht="15" thickBot="1">
+    <row r="133" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z133" s="23" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="134" spans="26:26" ht="15" thickBot="1">
+    <row r="134" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z134" s="23" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="135" spans="26:26" ht="15" thickBot="1">
+    <row r="135" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z135" s="23" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="136" spans="26:26" ht="15" thickBot="1">
+    <row r="136" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z136" s="23" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="137" spans="26:26" ht="15" thickBot="1">
+    <row r="137" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z137" s="23" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="138" spans="26:26" ht="15" thickBot="1">
+    <row r="138" spans="26:26" ht="15.75" thickBot="1">
       <c r="Z138" s="23" t="s">
         <v>210</v>
       </c>
@@ -2299,24 +2299,24 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="26.1796875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="17.54296875" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="27.90625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="15.36328125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="19.90625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="15.36328125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="15.54296875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="27.85546875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="5" customFormat="1">
@@ -2711,14 +2711,14 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="3.90625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" customWidth="1"/>
-    <col min="12" max="12" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="5:13">

</xml_diff>

<commit_message>
Final Fix for GUI
</commit_message>
<xml_diff>
--- a/Input_sheet_V2.xlsx
+++ b/Input_sheet_V2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Execution_Sheet" sheetId="5" r:id="rId1"/>
@@ -933,9 +933,6 @@
     <t>10.95.213.132</t>
   </si>
   <si>
-    <t>CCNtasuser@123</t>
-  </si>
-  <si>
     <t>/cluster/storage/no-backup/ccn/CcnStorage0/CCNCDR44/archive/</t>
   </si>
   <si>
@@ -943,6 +940,9 @@
   </si>
   <si>
     <t>/cluster/storage/no-backup/ccn/CcnStorage1/CCNCDR44/archive/</t>
+  </si>
+  <si>
+    <t>tasuserCCN@123 </t>
   </si>
 </sst>
 </file>
@@ -1481,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1493,7 +1493,7 @@
     <col min="4" max="4" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.54296875" style="11" customWidth="1"/>
-    <col min="7" max="7" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.81640625" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.81640625" customWidth="1"/>
@@ -3726,8 +3726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3870,10 +3870,10 @@
         <v>292</v>
       </c>
       <c r="D7" t="s">
+        <v>308</v>
+      </c>
+      <c r="E7" t="s">
         <v>305</v>
-      </c>
-      <c r="E7" t="s">
-        <v>306</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -3881,7 +3881,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B8" t="s">
         <v>304</v>
@@ -3890,10 +3890,10 @@
         <v>292</v>
       </c>
       <c r="D8" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -3901,5 +3901,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>